<commit_message>
updated land use data, updated start year calibration 2020
</commit_message>
<xml_diff>
--- a/InputData/land/BLAPE/BAU LULUCF Anthro Pollutant Emis.xlsx
+++ b/InputData/land/BLAPE/BAU LULUCF Anthro Pollutant Emis.xlsx
@@ -1,28 +1,63 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Meghan\Dropbox (Energy Innovation)\EPS Versions\eps-1.5.0-us-wipL\InputData\land\BLAPE\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\olivia\Documents\EPS_Models by Region\United States\NEW_US\InputData\land\BLAPE\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B2179FD-F64B-44FA-A408-E63036BE5F30}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="390" yWindow="90" windowWidth="19140" windowHeight="9270"/>
+    <workbookView xWindow="1470" yWindow="1680" windowWidth="13620" windowHeight="13320" firstSheet="2" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
-    <sheet name="Data" sheetId="2" r:id="rId2"/>
-    <sheet name="data from RPEpUACE" sheetId="4" r:id="rId3"/>
-    <sheet name="BLAPE" sheetId="3" r:id="rId4"/>
+    <sheet name="Calcs" sheetId="2" r:id="rId2"/>
+    <sheet name="EPA Table 6-1" sheetId="5" r:id="rId3"/>
+    <sheet name="data from RPEpUACE" sheetId="4" r:id="rId4"/>
+    <sheet name="BLAPE" sheetId="3" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="1">
+    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLDAPR" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <cellMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </cellMetadata>
+</metadata>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="54">
   <si>
     <t>Source:</t>
   </si>
@@ -144,9 +179,6 @@
     <t>F gases</t>
   </si>
   <si>
-    <t>CO2 Sequestration</t>
-  </si>
-  <si>
     <t>Rebound CH4 and N2O Emissions</t>
   </si>
   <si>
@@ -154,12 +186,45 @@
   </si>
   <si>
     <t>Projected pollutant emissions data for the land use sector until 2030, linearly extrapolated to 2050</t>
+  </si>
+  <si>
+    <t>Table 6-1</t>
+  </si>
+  <si>
+    <t>LULUCF Carbon Stock Change</t>
+  </si>
+  <si>
+    <t>EPS</t>
+  </si>
+  <si>
+    <t>Start Year Forecast</t>
+  </si>
+  <si>
+    <t>MMTCO2e</t>
+  </si>
+  <si>
+    <t>CO2 Sequestration Forecast</t>
+  </si>
+  <si>
+    <t>CO2 Sequestration Start Year</t>
+  </si>
+  <si>
+    <t>US EPA</t>
+  </si>
+  <si>
+    <t>https://www.epa.gov/sites/production/files/2021-02/documents/us-ghg-inventory-2021-main-text.pdf</t>
+  </si>
+  <si>
+    <t>Draft Inventory of US Greenhouse Gas Emissions Emissions and Sinks</t>
+  </si>
+  <si>
+    <t>Table 6-1, page 6-3 (467)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -193,7 +258,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -209,6 +274,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -235,7 +306,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
@@ -255,6 +326,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -349,6 +423,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -384,6 +475,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -559,109 +667,144 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B14"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:B21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.3984375" customWidth="1"/>
-    <col min="2" max="2" width="51.59765625" customWidth="1"/>
+    <col min="1" max="1" width="9.42578125" customWidth="1"/>
+    <col min="2" max="2" width="51.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B3" s="13" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B5" s="6">
         <v>2016</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B7" s="2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B10" s="13" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="6">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B14" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B17" s="13" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B18" s="14" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="B11" s="14" t="s">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A13" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A14" t="s">
-        <v>43</v>
-      </c>
-    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B7" r:id="rId1" xr:uid="{A4341B2F-D9AB-49A2-AA50-5B7AD476C902}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F10"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:G13"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="36.3984375" customWidth="1"/>
+    <col min="1" max="1" width="63.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B3">
         <v>2015</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="15">
         <v>2020</v>
       </c>
       <c r="D3">
@@ -674,15 +817,16 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>1</v>
       </c>
       <c r="B4">
         <v>-970</v>
       </c>
-      <c r="C4">
-        <v>-1191</v>
+      <c r="C4" s="15">
+        <f>G13</f>
+        <v>-818.39999999999986</v>
       </c>
       <c r="D4">
         <v>-1201</v>
@@ -692,18 +836,19 @@
       </c>
       <c r="F4" s="9">
         <f>TREND($B4:$E4,$B$3:$E$3,F$3)</f>
-        <v>-1369.7000000000007</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
+        <v>-1481.4799999999959</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>2</v>
       </c>
       <c r="B5">
         <v>-928</v>
       </c>
-      <c r="C5">
-        <v>-1044</v>
+      <c r="C5" s="15">
+        <f>G13</f>
+        <v>-818.39999999999986</v>
       </c>
       <c r="D5">
         <v>-908</v>
@@ -713,10 +858,10 @@
       </c>
       <c r="F5" s="9">
         <f>TREND($B5:$E5,$B$3:$E$3,F$3)</f>
-        <v>-423.09999999999854</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
+        <v>-490.77999999999884</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>4</v>
       </c>
@@ -726,7 +871,7 @@
       </c>
       <c r="C7" s="7">
         <f t="shared" si="0"/>
-        <v>-1117.5</v>
+        <v>-818.39999999999986</v>
       </c>
       <c r="D7" s="7">
         <f t="shared" si="0"/>
@@ -738,17 +883,74 @@
       </c>
       <c r="F7" s="7">
         <f t="shared" si="0"/>
-        <v>-896.39999999999964</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.45">
+        <v>-986.12999999999738</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>7</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G11" s="16" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>45</v>
+      </c>
+      <c r="B12">
+        <v>2015</v>
+      </c>
+      <c r="C12">
+        <v>2016</v>
+      </c>
+      <c r="D12">
+        <v>2017</v>
+      </c>
+      <c r="E12">
+        <v>2018</v>
+      </c>
+      <c r="F12">
+        <v>2019</v>
+      </c>
+      <c r="G12" s="15">
+        <v>2020</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>47</v>
+      </c>
+      <c r="B13">
+        <f>'EPA Table 6-1'!D2</f>
+        <v>-791.5</v>
+      </c>
+      <c r="C13">
+        <f>'EPA Table 6-1'!E2</f>
+        <v>-855.8</v>
+      </c>
+      <c r="D13">
+        <f>'EPA Table 6-1'!F2</f>
+        <v>-791.8</v>
+      </c>
+      <c r="E13">
+        <f>'EPA Table 6-1'!G2</f>
+        <v>-824.6</v>
+      </c>
+      <c r="F13">
+        <f>'EPA Table 6-1'!H2</f>
+        <v>-812.4</v>
+      </c>
+      <c r="G13" s="15" cm="1">
+        <f t="array" ref="G13">TREND(B13:F13,B12:F12,G12)</f>
+        <v>-818.39999999999986</v>
       </c>
     </row>
   </sheetData>
@@ -760,22 +962,93 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{748C1EED-5369-4626-8108-4C2C32A7C6AB}">
+  <dimension ref="A1:H2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="21.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B1">
+        <v>1990</v>
+      </c>
+      <c r="C1">
+        <v>2005</v>
+      </c>
+      <c r="D1">
+        <v>2015</v>
+      </c>
+      <c r="E1">
+        <v>2016</v>
+      </c>
+      <c r="F1">
+        <v>2017</v>
+      </c>
+      <c r="G1">
+        <v>2018</v>
+      </c>
+      <c r="H1">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B2">
+        <v>-908.7</v>
+      </c>
+      <c r="C2">
+        <v>-804.8</v>
+      </c>
+      <c r="D2">
+        <v>-791.5</v>
+      </c>
+      <c r="E2">
+        <v>-855.8</v>
+      </c>
+      <c r="F2">
+        <v>-791.8</v>
+      </c>
+      <c r="G2">
+        <v>-824.6</v>
+      </c>
+      <c r="H2">
+        <v>-812.4</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:B13"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="23" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B1" s="12" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>28</v>
       </c>
@@ -783,7 +1056,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>29</v>
       </c>
@@ -791,7 +1064,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>30</v>
       </c>
@@ -799,7 +1072,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>31</v>
       </c>
@@ -807,7 +1080,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>32</v>
       </c>
@@ -815,7 +1088,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>33</v>
       </c>
@@ -823,7 +1096,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>34</v>
       </c>
@@ -831,7 +1104,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>35</v>
       </c>
@@ -839,7 +1112,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>36</v>
       </c>
@@ -847,7 +1120,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>37</v>
       </c>
@@ -855,7 +1128,7 @@
         <v>4.2997168577917945E-4</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>38</v>
       </c>
@@ -863,7 +1136,7 @@
         <v>3.5003753313133949E-5</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>39</v>
       </c>
@@ -876,22 +1149,24 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <sheetPr>
     <tabColor theme="3"/>
   </sheetPr>
   <dimension ref="A1:AK13"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.73046875" customWidth="1"/>
-    <col min="2" max="17" width="11.265625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.7109375" customWidth="1"/>
+    <col min="2" max="17" width="11.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:37" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>8</v>
       </c>
@@ -1004,156 +1279,156 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="2" spans="1:37" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>16</v>
       </c>
       <c r="B2" s="4">
-        <f>TREND(Data!$B7:$C7,Data!$B3:$C3,BLAPE!B1)*10^12</f>
-        <v>-949000000000000</v>
+        <f>TREND(Calcs!$B7:$C7,Calcs!$B3:$C3,BLAPE!B1)*10^12</f>
+        <v>-948999999999992.75</v>
       </c>
       <c r="C2" s="4">
-        <f>TREND(Data!$B7:$C7,Data!$B3:$C3,BLAPE!C1)*10^12</f>
-        <v>-982700000000011.63</v>
+        <f>TREND(Calcs!$B7:$C7,Calcs!$B3:$C3,BLAPE!C1)*10^12</f>
+        <v>-922879999999997.38</v>
       </c>
       <c r="D2" s="4">
-        <f>TREND(Data!$B7:$C7,Data!$B3:$C3,BLAPE!D1)*10^12</f>
-        <v>-1016400000000008.8</v>
+        <f>TREND(Calcs!$B7:$C7,Calcs!$B3:$C3,BLAPE!D1)*10^12</f>
+        <v>-896759999999994.75</v>
       </c>
       <c r="E2" s="4">
-        <f>TREND(Data!$B7:$C7,Data!$B3:$C3,BLAPE!E1)*10^12</f>
-        <v>-1050100000000005.9</v>
+        <f>TREND(Calcs!$B7:$C7,Calcs!$B3:$C3,BLAPE!E1)*10^12</f>
+        <v>-870639999999992.13</v>
       </c>
       <c r="F2" s="4">
-        <f>TREND(Data!$B7:$C7,Data!$B3:$C3,BLAPE!F1)*10^12</f>
-        <v>-1083800000000002.9</v>
+        <f>TREND(Calcs!$B7:$C7,Calcs!$B3:$C3,BLAPE!F1)*10^12</f>
+        <v>-844519999999996.75</v>
       </c>
       <c r="G2" s="5">
-        <f>TREND(Data!$B7:$C7,Data!$B3:$C3,BLAPE!G1)*10^12</f>
-        <v>-1117500000000000</v>
+        <f>TREND(Calcs!$B7:$C7,Calcs!$B3:$C3,BLAPE!G1)*10^12</f>
+        <v>-818399999999994.13</v>
       </c>
       <c r="H2" s="4">
-        <f>TREND(Data!$C7:$D7,Data!$C3:$D3,BLAPE!H1)*10^12</f>
-        <v>-1104900000000001.5</v>
+        <f>TREND(Calcs!$C7:$D7,Calcs!$C3:$D3,BLAPE!H1)*10^12</f>
+        <v>-865619999999995.38</v>
       </c>
       <c r="I2" s="4">
-        <f>TREND(Data!$C7:$D7,Data!$C3:$D3,BLAPE!I1)*10^12</f>
-        <v>-1092299999999999.3</v>
+        <f>TREND(Calcs!$C7:$D7,Calcs!$C3:$D3,BLAPE!I1)*10^12</f>
+        <v>-912839999999996.5</v>
       </c>
       <c r="J2" s="4">
-        <f>TREND(Data!$C7:$D7,Data!$C3:$D3,BLAPE!J1)*10^12</f>
-        <v>-1079700000000000.8</v>
+        <f>TREND(Calcs!$C7:$D7,Calcs!$C3:$D3,BLAPE!J1)*10^12</f>
+        <v>-960059999999997.63</v>
       </c>
       <c r="K2" s="4">
-        <f>TREND(Data!$C7:$D7,Data!$C3:$D3,BLAPE!K1)*10^12</f>
-        <v>-1067100000000002.1</v>
+        <f>TREND(Calcs!$C7:$D7,Calcs!$C3:$D3,BLAPE!K1)*10^12</f>
+        <v>-1007279999999998.9</v>
       </c>
       <c r="L2" s="5">
-        <f>TREND(Data!$C7:$D7,Data!$C3:$D3,BLAPE!L1)*10^12</f>
+        <f>TREND(Calcs!$C7:$D7,Calcs!$C3:$D3,BLAPE!L1)*10^12</f>
         <v>-1054500000000000</v>
       </c>
       <c r="M2" s="4">
-        <f>TREND(Data!$D7:$E7,Data!$D3:$E3,BLAPE!M1)*10^12</f>
+        <f>TREND(Calcs!$D7:$E7,Calcs!$D3:$E3,BLAPE!M1)*10^12</f>
         <v>-1024300000000002.9</v>
       </c>
       <c r="N2" s="4">
-        <f>TREND(Data!$D7:$E7,Data!$D3:$E3,BLAPE!N1)*10^12</f>
+        <f>TREND(Calcs!$D7:$E7,Calcs!$D3:$E3,BLAPE!N1)*10^12</f>
         <v>-994099999999998.5</v>
       </c>
       <c r="O2" s="4">
-        <f>TREND(Data!$D7:$E7,Data!$D3:$E3,BLAPE!O1)*10^12</f>
+        <f>TREND(Calcs!$D7:$E7,Calcs!$D3:$E3,BLAPE!O1)*10^12</f>
         <v>-963900000000001.5</v>
       </c>
       <c r="P2" s="4">
-        <f>TREND(Data!$D7:$E7,Data!$D3:$E3,BLAPE!P1)*10^12</f>
+        <f>TREND(Calcs!$D7:$E7,Calcs!$D3:$E3,BLAPE!P1)*10^12</f>
         <v>-933700000000004.38</v>
       </c>
       <c r="Q2" s="5">
-        <f>TREND(Data!$D7:$E7,Data!$D3:$E3,BLAPE!Q1)*10^12</f>
+        <f>TREND(Calcs!$D7:$E7,Calcs!$D3:$E3,BLAPE!Q1)*10^12</f>
         <v>-903500000000000</v>
       </c>
       <c r="R2" s="4">
-        <f>TREND(Data!$E7:$F7,Data!$E3:$F3,BLAPE!R1)*10^12</f>
-        <v>-903144999999999.88</v>
+        <f>TREND(Calcs!$E7:$F7,Calcs!$E3:$F3,BLAPE!R1)*10^12</f>
+        <v>-907631500000001.38</v>
       </c>
       <c r="S2" s="4">
-        <f>TREND(Data!$E7:$F7,Data!$E3:$F3,BLAPE!S1)*10^12</f>
-        <v>-902789999999999.88</v>
+        <f>TREND(Calcs!$E7:$F7,Calcs!$E3:$F3,BLAPE!S1)*10^12</f>
+        <v>-911763000000000.88</v>
       </c>
       <c r="T2" s="4">
-        <f>TREND(Data!$E7:$F7,Data!$E3:$F3,BLAPE!T1)*10^12</f>
-        <v>-902434999999999.88</v>
+        <f>TREND(Calcs!$E7:$F7,Calcs!$E3:$F3,BLAPE!T1)*10^12</f>
+        <v>-915894500000000.38</v>
       </c>
       <c r="U2" s="4">
-        <f>TREND(Data!$E7:$F7,Data!$E3:$F3,BLAPE!U1)*10^12</f>
-        <v>-902079999999999.88</v>
+        <f>TREND(Calcs!$E7:$F7,Calcs!$E3:$F3,BLAPE!U1)*10^12</f>
+        <v>-920025999999999.88</v>
       </c>
       <c r="V2" s="11">
-        <f>TREND(Data!$E7:$F7,Data!$E3:$F3,BLAPE!V1)*10^12</f>
-        <v>-901724999999999.75</v>
+        <f>TREND(Calcs!$E7:$F7,Calcs!$E3:$F3,BLAPE!V1)*10^12</f>
+        <v>-924157499999999.38</v>
       </c>
       <c r="W2" s="11">
-        <f>TREND(Data!$E7:$F7,Data!$E3:$F3,BLAPE!W1)*10^12</f>
-        <v>-901369999999999.75</v>
+        <f>TREND(Calcs!$E7:$F7,Calcs!$E3:$F3,BLAPE!W1)*10^12</f>
+        <v>-928289000000000.63</v>
       </c>
       <c r="X2" s="4">
-        <f>TREND(Data!$E7:$F7,Data!$E3:$F3,BLAPE!X1)*10^12</f>
-        <v>-901014999999999.75</v>
+        <f>TREND(Calcs!$E7:$F7,Calcs!$E3:$F3,BLAPE!X1)*10^12</f>
+        <v>-932420500000000.13</v>
       </c>
       <c r="Y2" s="4">
-        <f>TREND(Data!$E7:$F7,Data!$E3:$F3,BLAPE!Y1)*10^12</f>
-        <v>-900659999999999.75</v>
+        <f>TREND(Calcs!$E7:$F7,Calcs!$E3:$F3,BLAPE!Y1)*10^12</f>
+        <v>-936551999999999.63</v>
       </c>
       <c r="Z2" s="4">
-        <f>TREND(Data!$E7:$F7,Data!$E3:$F3,BLAPE!Z1)*10^12</f>
-        <v>-900304999999999.75</v>
+        <f>TREND(Calcs!$E7:$F7,Calcs!$E3:$F3,BLAPE!Z1)*10^12</f>
+        <v>-940683499999999.13</v>
       </c>
       <c r="AA2" s="4">
-        <f>TREND(Data!$E7:$F7,Data!$E3:$F3,BLAPE!AA1)*10^12</f>
-        <v>-899949999999999.75</v>
+        <f>TREND(Calcs!$E7:$F7,Calcs!$E3:$F3,BLAPE!AA1)*10^12</f>
+        <v>-944814999999998.75</v>
       </c>
       <c r="AB2" s="4">
-        <f>TREND(Data!$E7:$F7,Data!$E3:$F3,BLAPE!AB1)*10^12</f>
-        <v>-899594999999999.63</v>
+        <f>TREND(Calcs!$E7:$F7,Calcs!$E3:$F3,BLAPE!AB1)*10^12</f>
+        <v>-948946500000000</v>
       </c>
       <c r="AC2" s="4">
-        <f>TREND(Data!$E7:$F7,Data!$E3:$F3,BLAPE!AC1)*10^12</f>
-        <v>-899239999999999.63</v>
+        <f>TREND(Calcs!$E7:$F7,Calcs!$E3:$F3,BLAPE!AC1)*10^12</f>
+        <v>-953077999999999.5</v>
       </c>
       <c r="AD2" s="4">
-        <f>TREND(Data!$E7:$F7,Data!$E3:$F3,BLAPE!AD1)*10^12</f>
-        <v>-898884999999999.63</v>
+        <f>TREND(Calcs!$E7:$F7,Calcs!$E3:$F3,BLAPE!AD1)*10^12</f>
+        <v>-957209499999999</v>
       </c>
       <c r="AE2" s="4">
-        <f>TREND(Data!$E7:$F7,Data!$E3:$F3,BLAPE!AE1)*10^12</f>
-        <v>-898529999999999.63</v>
+        <f>TREND(Calcs!$E7:$F7,Calcs!$E3:$F3,BLAPE!AE1)*10^12</f>
+        <v>-961340999999998.5</v>
       </c>
       <c r="AF2" s="4">
-        <f>TREND(Data!$E7:$F7,Data!$E3:$F3,BLAPE!AF1)*10^12</f>
-        <v>-898174999999999.63</v>
+        <f>TREND(Calcs!$E7:$F7,Calcs!$E3:$F3,BLAPE!AF1)*10^12</f>
+        <v>-965472499999998</v>
       </c>
       <c r="AG2" s="4">
-        <f>TREND(Data!$E7:$F7,Data!$E3:$F3,BLAPE!AG1)*10^12</f>
-        <v>-897819999999999.63</v>
+        <f>TREND(Calcs!$E7:$F7,Calcs!$E3:$F3,BLAPE!AG1)*10^12</f>
+        <v>-969603999999999.38</v>
       </c>
       <c r="AH2" s="4">
-        <f>TREND(Data!$E7:$F7,Data!$E3:$F3,BLAPE!AH1)*10^12</f>
-        <v>-897464999999999.63</v>
+        <f>TREND(Calcs!$E7:$F7,Calcs!$E3:$F3,BLAPE!AH1)*10^12</f>
+        <v>-973735499999998.88</v>
       </c>
       <c r="AI2" s="4">
-        <f>TREND(Data!$E7:$F7,Data!$E3:$F3,BLAPE!AI1)*10^12</f>
-        <v>-897109999999999.5</v>
+        <f>TREND(Calcs!$E7:$F7,Calcs!$E3:$F3,BLAPE!AI1)*10^12</f>
+        <v>-977866999999998.38</v>
       </c>
       <c r="AJ2" s="4">
-        <f>TREND(Data!$E7:$F7,Data!$E3:$F3,BLAPE!AJ1)*10^12</f>
-        <v>-896754999999999.5</v>
+        <f>TREND(Calcs!$E7:$F7,Calcs!$E3:$F3,BLAPE!AJ1)*10^12</f>
+        <v>-981998499999997.88</v>
       </c>
       <c r="AK2" s="4">
-        <f>TREND(Data!$E7:$F7,Data!$E3:$F3,BLAPE!AK1)*10^12</f>
-        <v>-896399999999999.5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:37" x14ac:dyDescent="0.45">
+        <f>TREND(Calcs!$E7:$F7,Calcs!$E3:$F3,BLAPE!AK1)*10^12</f>
+        <v>-986129999999997.38</v>
+      </c>
+    </row>
+    <row r="3" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>17</v>
       </c>
@@ -1266,7 +1541,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:37" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>18</v>
       </c>
@@ -1379,7 +1654,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:37" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>19</v>
       </c>
@@ -1492,7 +1767,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:37" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>20</v>
       </c>
@@ -1605,7 +1880,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:37" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>21</v>
       </c>
@@ -1718,7 +1993,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:37" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>22</v>
       </c>
@@ -1831,7 +2106,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:37" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>23</v>
       </c>
@@ -1944,7 +2219,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:37" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>24</v>
       </c>
@@ -2057,49 +2332,49 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:37" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>25</v>
       </c>
       <c r="B11" s="4">
         <f>B$2*-'data from RPEpUACE'!$B11</f>
-        <v>408043129804.44128</v>
+        <v>408043129804.43817</v>
       </c>
       <c r="C11" s="4">
         <f>C$2*-'data from RPEpUACE'!$B11</f>
-        <v>422533175615.20465</v>
+        <v>396812269371.888</v>
       </c>
       <c r="D11" s="4">
         <f>D$2*-'data from RPEpUACE'!$B11</f>
-        <v>437023221425.96173</v>
+        <v>385581408939.33472</v>
       </c>
       <c r="E11" s="4">
         <f>E$2*-'data from RPEpUACE'!$B11</f>
-        <v>451513267236.71887</v>
+        <v>374350548506.78143</v>
       </c>
       <c r="F11" s="4">
         <f>F$2*-'data from RPEpUACE'!$B11</f>
-        <v>466003313047.47595</v>
+        <v>363119688074.2312</v>
       </c>
       <c r="G11" s="4">
         <f>G$2*-'data from RPEpUACE'!$B11</f>
-        <v>480493358858.23303</v>
+        <v>351888827641.67792</v>
       </c>
       <c r="H11" s="4">
         <f>H$2*-'data from RPEpUACE'!$B11</f>
-        <v>475075715617.41602</v>
+        <v>372192090644.17133</v>
       </c>
       <c r="I11" s="4">
         <f>I$2*-'data from RPEpUACE'!$B11</f>
-        <v>469658072376.59741</v>
+        <v>392495353646.66467</v>
       </c>
       <c r="J11" s="4">
         <f>J$2*-'data from RPEpUACE'!$B11</f>
-        <v>464240429135.7804</v>
+        <v>412798616649.15802</v>
       </c>
       <c r="K11" s="4">
         <f>K$2*-'data from RPEpUACE'!$B11</f>
-        <v>458822785894.96332</v>
+        <v>433101879651.65137</v>
       </c>
       <c r="L11" s="4">
         <f>L$2*-'data from RPEpUACE'!$B11</f>
@@ -2127,128 +2402,128 @@
       </c>
       <c r="R11" s="4">
         <f>R$2*-'data from RPEpUACE'!$B11</f>
-        <v>388326778153.03699</v>
+        <v>390255846121.28589</v>
       </c>
       <c r="S11" s="4">
         <f>S$2*-'data from RPEpUACE'!$B11</f>
-        <v>388174138204.58539</v>
+        <v>392032274141.0824</v>
       </c>
       <c r="T11" s="4">
         <f>T$2*-'data from RPEpUACE'!$B11</f>
-        <v>388021498256.13373</v>
+        <v>393808702160.87885</v>
       </c>
       <c r="U11" s="4">
         <f>U$2*-'data from RPEpUACE'!$B11</f>
-        <v>387868858307.68213</v>
+        <v>395585130180.67529</v>
       </c>
       <c r="V11" s="4">
         <f>V$2*-'data from RPEpUACE'!$B11</f>
-        <v>387716218359.23047</v>
+        <v>397361558200.47174</v>
       </c>
       <c r="W11" s="4">
         <f>W$2*-'data from RPEpUACE'!$B11</f>
-        <v>387563578410.77887</v>
+        <v>399137986220.26898</v>
       </c>
       <c r="X11" s="4">
         <f>X$2*-'data from RPEpUACE'!$B11</f>
-        <v>387410938462.32727</v>
+        <v>400914414240.06543</v>
       </c>
       <c r="Y11" s="4">
         <f>Y$2*-'data from RPEpUACE'!$B11</f>
-        <v>387258298513.87567</v>
+        <v>402690842259.86194</v>
       </c>
       <c r="Z11" s="4">
         <f>Z$2*-'data from RPEpUACE'!$B11</f>
-        <v>387105658565.42407</v>
+        <v>404467270279.65839</v>
       </c>
       <c r="AA11" s="4">
         <f>AA$2*-'data from RPEpUACE'!$B11</f>
-        <v>386953018616.97241</v>
+        <v>406243698299.4549</v>
       </c>
       <c r="AB11" s="4">
         <f>AB$2*-'data from RPEpUACE'!$B11</f>
-        <v>386800378668.52075</v>
+        <v>408020126319.25214</v>
       </c>
       <c r="AC11" s="4">
         <f>AC$2*-'data from RPEpUACE'!$B11</f>
-        <v>386647738720.06915</v>
+        <v>409796554339.04858</v>
       </c>
       <c r="AD11" s="4">
         <f>AD$2*-'data from RPEpUACE'!$B11</f>
-        <v>386495098771.61755</v>
+        <v>411572982358.84503</v>
       </c>
       <c r="AE11" s="4">
         <f>AE$2*-'data from RPEpUACE'!$B11</f>
-        <v>386342458823.16595</v>
+        <v>413349410378.64148</v>
       </c>
       <c r="AF11" s="4">
         <f>AF$2*-'data from RPEpUACE'!$B11</f>
-        <v>386189818874.71436</v>
+        <v>415125838398.43799</v>
       </c>
       <c r="AG11" s="4">
         <f>AG$2*-'data from RPEpUACE'!$B11</f>
-        <v>386037178926.26276</v>
+        <v>416902266418.23523</v>
       </c>
       <c r="AH11" s="4">
         <f>AH$2*-'data from RPEpUACE'!$B11</f>
-        <v>385884538977.8111</v>
+        <v>418678694438.03168</v>
       </c>
       <c r="AI11" s="4">
         <f>AI$2*-'data from RPEpUACE'!$B11</f>
-        <v>385731899029.35944</v>
+        <v>420455122457.82819</v>
       </c>
       <c r="AJ11" s="4">
         <f>AJ$2*-'data from RPEpUACE'!$B11</f>
-        <v>385579259080.90784</v>
+        <v>422231550477.62463</v>
       </c>
       <c r="AK11" s="4">
         <f>AK$2*-'data from RPEpUACE'!$B11</f>
-        <v>385426619132.45624</v>
-      </c>
-    </row>
-    <row r="12" spans="1:37" x14ac:dyDescent="0.45">
+        <v>424007978497.42108</v>
+      </c>
+    </row>
+    <row r="12" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>26</v>
       </c>
       <c r="B12" s="4">
         <f>B$2*-'data from RPEpUACE'!$B12</f>
-        <v>33218561894.164116</v>
+        <v>33218561894.163864</v>
       </c>
       <c r="C12" s="4">
         <f>C$2*-'data from RPEpUACE'!$B12</f>
-        <v>34398188380.817139</v>
+        <v>32304263857.624966</v>
       </c>
       <c r="D12" s="4">
         <f>D$2*-'data from RPEpUACE'!$B12</f>
-        <v>35577814867.46965</v>
+        <v>31389965821.085815</v>
       </c>
       <c r="E12" s="4">
         <f>E$2*-'data from RPEpUACE'!$B12</f>
-        <v>36757441354.122162</v>
+        <v>30475667784.546665</v>
       </c>
       <c r="F12" s="4">
         <f>F$2*-'data from RPEpUACE'!$B12</f>
-        <v>37937067840.774673</v>
+        <v>29561369748.007767</v>
       </c>
       <c r="G12" s="4">
         <f>G$2*-'data from RPEpUACE'!$B12</f>
-        <v>39116694327.427185</v>
+        <v>28647071711.468616</v>
       </c>
       <c r="H12" s="4">
         <f>H$2*-'data from RPEpUACE'!$B12</f>
-        <v>38675647035.681755</v>
+        <v>30299948942.914848</v>
       </c>
       <c r="I12" s="4">
         <f>I$2*-'data from RPEpUACE'!$B12</f>
-        <v>38234599743.936188</v>
+        <v>31952826174.361073</v>
       </c>
       <c r="J12" s="4">
         <f>J$2*-'data from RPEpUACE'!$B12</f>
-        <v>37793552452.19075</v>
+        <v>33605703405.807297</v>
       </c>
       <c r="K12" s="4">
         <f>K$2*-'data from RPEpUACE'!$B12</f>
-        <v>37352505160.445313</v>
+        <v>35258580637.253525</v>
       </c>
       <c r="L12" s="4">
         <f>L$2*-'data from RPEpUACE'!$B12</f>
@@ -2276,86 +2551,86 @@
       </c>
       <c r="R12" s="4">
         <f>R$2*-'data from RPEpUACE'!$B12</f>
-        <v>31613464785.990356</v>
+        <v>31770509125.229782</v>
       </c>
       <c r="S12" s="4">
         <f>S$2*-'data from RPEpUACE'!$B12</f>
-        <v>31601038453.564194</v>
+        <v>31915127132.04298</v>
       </c>
       <c r="T12" s="4">
         <f>T$2*-'data from RPEpUACE'!$B12</f>
-        <v>31588612121.138031</v>
+        <v>32059745138.856174</v>
       </c>
       <c r="U12" s="4">
         <f>U$2*-'data from RPEpUACE'!$B12</f>
-        <v>31576185788.711868</v>
+        <v>32204363145.669369</v>
       </c>
       <c r="V12" s="4">
         <f>V$2*-'data from RPEpUACE'!$B12</f>
-        <v>31563759456.285702</v>
+        <v>32348981152.482567</v>
       </c>
       <c r="W12" s="4">
         <f>W$2*-'data from RPEpUACE'!$B12</f>
-        <v>31551333123.859539</v>
+        <v>32493599159.295822</v>
       </c>
       <c r="X12" s="4">
         <f>X$2*-'data from RPEpUACE'!$B12</f>
-        <v>31538906791.433376</v>
+        <v>32638217166.109016</v>
       </c>
       <c r="Y12" s="4">
         <f>Y$2*-'data from RPEpUACE'!$B12</f>
-        <v>31526480459.007214</v>
+        <v>32782835172.922215</v>
       </c>
       <c r="Z12" s="4">
         <f>Z$2*-'data from RPEpUACE'!$B12</f>
-        <v>31514054126.581051</v>
+        <v>32927453179.735409</v>
       </c>
       <c r="AA12" s="4">
         <f>AA$2*-'data from RPEpUACE'!$B12</f>
-        <v>31501627794.154888</v>
+        <v>33072071186.548607</v>
       </c>
       <c r="AB12" s="4">
         <f>AB$2*-'data from RPEpUACE'!$B12</f>
-        <v>31489201461.728722</v>
+        <v>33216689193.361866</v>
       </c>
       <c r="AC12" s="4">
         <f>AC$2*-'data from RPEpUACE'!$B12</f>
-        <v>31476775129.302559</v>
+        <v>33361307200.17506</v>
       </c>
       <c r="AD12" s="4">
         <f>AD$2*-'data from RPEpUACE'!$B12</f>
-        <v>31464348796.876396</v>
+        <v>33505925206.988255</v>
       </c>
       <c r="AE12" s="4">
         <f>AE$2*-'data from RPEpUACE'!$B12</f>
-        <v>31451922464.450233</v>
+        <v>33650543213.801453</v>
       </c>
       <c r="AF12" s="4">
         <f>AF$2*-'data from RPEpUACE'!$B12</f>
-        <v>31439496132.024071</v>
+        <v>33795161220.614647</v>
       </c>
       <c r="AG12" s="4">
         <f>AG$2*-'data from RPEpUACE'!$B12</f>
-        <v>31427069799.597908</v>
+        <v>33939779227.427906</v>
       </c>
       <c r="AH12" s="4">
         <f>AH$2*-'data from RPEpUACE'!$B12</f>
-        <v>31414643467.171745</v>
+        <v>34084397234.241104</v>
       </c>
       <c r="AI12" s="4">
         <f>AI$2*-'data from RPEpUACE'!$B12</f>
-        <v>31402217134.745579</v>
+        <v>34229015241.054298</v>
       </c>
       <c r="AJ12" s="4">
         <f>AJ$2*-'data from RPEpUACE'!$B12</f>
-        <v>31389790802.319416</v>
+        <v>34373633247.867493</v>
       </c>
       <c r="AK12" s="4">
         <f>AK$2*-'data from RPEpUACE'!$B12</f>
-        <v>31377364469.893253</v>
-      </c>
-    </row>
-    <row r="13" spans="1:37" x14ac:dyDescent="0.45">
+        <v>34518251254.680687</v>
+      </c>
+    </row>
+    <row r="13" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>15</v>
       </c>

</xml_diff>

<commit_message>
Updates to BAU LULUCF emissions
Now take last 5 year trend instead of BUR projections
</commit_message>
<xml_diff>
--- a/InputData/land/BLAPE/BAU LULUCF Anthro Pollutant Emis.xlsx
+++ b/InputData/land/BLAPE/BAU LULUCF Anthro Pollutant Emis.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\olivia\Documents\EPS_Models by Region\United States\NEW_US\InputData\land\BLAPE\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rorvis\Dropbox (Energy InNovation)\My Documents\Energy Policy Solutions\US\Models\eps-us\InputData\land\BLAPE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B2179FD-F64B-44FA-A408-E63036BE5F30}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9B6FDE4-7C6E-4C9F-A4A8-79AB3428627D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1470" yWindow="1680" windowWidth="13620" windowHeight="13320" firstSheet="2" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -57,7 +57,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="50">
   <si>
     <t>Source:</t>
   </si>
@@ -86,21 +86,9 @@
     <t>Year</t>
   </si>
   <si>
-    <t>U.S. State Department</t>
-  </si>
-  <si>
     <t>Notes</t>
   </si>
   <si>
-    <t>Page 34, Table 3</t>
-  </si>
-  <si>
-    <t>https://unfccc.int/files/national_reports/biennial_reports_and_iar/submitted_biennial_reports/application/pdf/2016_second_biennial_report_of_the_united_states_.pdf</t>
-  </si>
-  <si>
-    <t>Second Biennial Report of the United States of America</t>
-  </si>
-  <si>
     <t>BLAPE BAU LULUCF Anthropogenic Pollutant Emissions</t>
   </si>
   <si>
@@ -185,9 +173,6 @@
     <t>See land/RPEpUACE</t>
   </si>
   <si>
-    <t>Projected pollutant emissions data for the land use sector until 2030, linearly extrapolated to 2050</t>
-  </si>
-  <si>
     <t>Table 6-1</t>
   </si>
   <si>
@@ -203,9 +188,6 @@
     <t>MMTCO2e</t>
   </si>
   <si>
-    <t>CO2 Sequestration Forecast</t>
-  </si>
-  <si>
     <t>CO2 Sequestration Start Year</t>
   </si>
   <si>
@@ -219,6 +201,12 @@
   </si>
   <si>
     <t>Table 6-1, page 6-3 (467)</t>
+  </si>
+  <si>
+    <t>We project the previous 5 years of LULUCF emissions forward to 2050.</t>
+  </si>
+  <si>
+    <t>These are relatively constant.</t>
   </si>
 </sst>
 </file>
@@ -306,7 +294,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
@@ -318,7 +306,6 @@
     </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="1" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -668,10 +655,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B21"/>
+  <dimension ref="A1:B22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -682,98 +669,74 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="13" t="s">
-        <v>48</v>
+      <c r="B3" s="12" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>9</v>
+        <v>44</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B5" s="6">
-        <v>2016</v>
+        <v>2021</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>13</v>
+        <v>46</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B7" s="2" t="s">
-        <v>12</v>
+        <v>45</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>11</v>
+        <v>47</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B10" s="13" t="s">
+      <c r="B10" s="12" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" s="16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="13" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" s="16" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="13" spans="1:2" s="16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B13"/>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="11" spans="1:2" s="17" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B11" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" s="17" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="6">
-        <v>2021</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" s="17" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B13" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B14" s="2" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B15" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B17" s="13" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B18" s="14" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>42</v>
-      </c>
-    </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="B7" r:id="rId1" xr:uid="{A4341B2F-D9AB-49A2-AA50-5B7AD476C902}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId2"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -782,7 +745,7 @@
   <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -804,7 +767,7 @@
       <c r="B3">
         <v>2015</v>
       </c>
-      <c r="C3" s="15">
+      <c r="C3" s="14">
         <v>2020</v>
       </c>
       <c r="D3">
@@ -824,19 +787,21 @@
       <c r="B4">
         <v>-970</v>
       </c>
-      <c r="C4" s="15">
+      <c r="C4" s="14">
         <f>G13</f>
         <v>-818.39999999999986</v>
       </c>
-      <c r="D4">
-        <v>-1201</v>
-      </c>
-      <c r="E4">
-        <v>-1118</v>
-      </c>
-      <c r="F4" s="9">
-        <f>TREND($B4:$E4,$B$3:$E$3,F$3)</f>
-        <v>-1481.4799999999959</v>
+      <c r="D4" cm="1">
+        <f t="array" ref="D4">TREND($B$13:$F$13,$B$12:$F$12,D3)</f>
+        <v>-823.7</v>
+      </c>
+      <c r="E4" cm="1">
+        <f t="array" ref="E4">TREND($B$13:$F$13,$B$12:$F$12,E3)</f>
+        <v>-829.00000000000023</v>
+      </c>
+      <c r="F4" cm="1">
+        <f t="array" ref="F4">TREND($B$13:$F$13,$B$12:$F$12,F3)</f>
+        <v>-850.2</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -846,19 +811,21 @@
       <c r="B5">
         <v>-928</v>
       </c>
-      <c r="C5" s="15">
+      <c r="C5" s="14">
         <f>G13</f>
         <v>-818.39999999999986</v>
       </c>
       <c r="D5">
-        <v>-908</v>
+        <f>D4</f>
+        <v>-823.7</v>
       </c>
       <c r="E5">
-        <v>-689</v>
-      </c>
-      <c r="F5" s="9">
-        <f>TREND($B5:$E5,$B$3:$E$3,F$3)</f>
-        <v>-490.77999999999884</v>
+        <f t="shared" ref="E5:F5" si="0">E4</f>
+        <v>-829.00000000000023</v>
+      </c>
+      <c r="F5">
+        <f t="shared" si="0"/>
+        <v>-850.2</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -866,24 +833,24 @@
         <v>4</v>
       </c>
       <c r="B7">
-        <f t="shared" ref="B7:F7" si="0">AVERAGE(B4:B5)</f>
+        <f t="shared" ref="B7:F7" si="1">AVERAGE(B4:B5)</f>
         <v>-949</v>
       </c>
       <c r="C7" s="7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-818.39999999999986</v>
       </c>
       <c r="D7" s="7">
-        <f t="shared" si="0"/>
-        <v>-1054.5</v>
+        <f t="shared" si="1"/>
+        <v>-823.7</v>
       </c>
       <c r="E7" s="7">
-        <f t="shared" si="0"/>
-        <v>-903.5</v>
+        <f t="shared" si="1"/>
+        <v>-829.00000000000023</v>
       </c>
       <c r="F7" s="7">
-        <f t="shared" si="0"/>
-        <v>-986.12999999999738</v>
+        <f t="shared" si="1"/>
+        <v>-850.2</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
@@ -897,13 +864,13 @@
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="G11" s="16" t="s">
-        <v>46</v>
+      <c r="G11" s="15" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="B12">
         <v>2015</v>
@@ -920,13 +887,13 @@
       <c r="F12">
         <v>2019</v>
       </c>
-      <c r="G12" s="15">
+      <c r="G12" s="14">
         <v>2020</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="B13">
         <f>'EPA Table 6-1'!D2</f>
@@ -948,7 +915,7 @@
         <f>'EPA Table 6-1'!H2</f>
         <v>-812.4</v>
       </c>
-      <c r="G13" s="15" cm="1">
+      <c r="G13" s="14" cm="1">
         <f t="array" ref="G13">TREND(B13:F13,B12:F12,G12)</f>
         <v>-818.39999999999986</v>
       </c>
@@ -976,7 +943,7 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="B1">
         <v>1990</v>
@@ -1002,7 +969,7 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="B2">
         <v>-908.7</v>
@@ -1044,13 +1011,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B1" s="12" t="s">
-        <v>27</v>
+      <c r="B1" s="11" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="B2">
         <v>0</v>
@@ -1058,7 +1025,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="B3">
         <v>0</v>
@@ -1066,7 +1033,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="B4">
         <v>0</v>
@@ -1074,7 +1041,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="B5">
         <v>0</v>
@@ -1082,7 +1049,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="B6">
         <v>0</v>
@@ -1090,7 +1057,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="B7">
         <v>0</v>
@@ -1098,7 +1065,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="B8">
         <v>0</v>
@@ -1106,7 +1073,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="B9">
         <v>0</v>
@@ -1114,7 +1081,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="B10">
         <v>0</v>
@@ -1122,7 +1089,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="B11" s="4">
         <v>4.2997168577917945E-4</v>
@@ -1130,7 +1097,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="B12" s="4">
         <v>3.5003753313133949E-5</v>
@@ -1138,7 +1105,7 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="B13">
         <v>0</v>
@@ -1156,8 +1123,8 @@
   </sheetPr>
   <dimension ref="A1:AK13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+    <sheetView topLeftCell="K1" workbookViewId="0">
+      <selection activeCell="AK2" sqref="AK2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1230,10 +1197,10 @@
       <c r="U1">
         <v>2034</v>
       </c>
-      <c r="V1" s="10">
+      <c r="V1" s="9">
         <v>2035</v>
       </c>
-      <c r="W1" s="10">
+      <c r="W1" s="9">
         <v>2036</v>
       </c>
       <c r="X1">
@@ -1281,7 +1248,7 @@
     </row>
     <row r="2" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="B2" s="4">
         <f>TREND(Calcs!$B7:$C7,Calcs!$B3:$C3,BLAPE!B1)*10^12</f>
@@ -1309,128 +1276,128 @@
       </c>
       <c r="H2" s="4">
         <f>TREND(Calcs!$C7:$D7,Calcs!$C3:$D3,BLAPE!H1)*10^12</f>
-        <v>-865619999999995.38</v>
+        <v>-819460000000000.25</v>
       </c>
       <c r="I2" s="4">
         <f>TREND(Calcs!$C7:$D7,Calcs!$C3:$D3,BLAPE!I1)*10^12</f>
-        <v>-912839999999996.5</v>
+        <v>-820520000000000.25</v>
       </c>
       <c r="J2" s="4">
         <f>TREND(Calcs!$C7:$D7,Calcs!$C3:$D3,BLAPE!J1)*10^12</f>
-        <v>-960059999999997.63</v>
+        <v>-821580000000000.13</v>
       </c>
       <c r="K2" s="4">
         <f>TREND(Calcs!$C7:$D7,Calcs!$C3:$D3,BLAPE!K1)*10^12</f>
-        <v>-1007279999999998.9</v>
+        <v>-822640000000000.13</v>
       </c>
       <c r="L2" s="5">
         <f>TREND(Calcs!$C7:$D7,Calcs!$C3:$D3,BLAPE!L1)*10^12</f>
-        <v>-1054500000000000</v>
+        <v>-823700000000000</v>
       </c>
       <c r="M2" s="4">
         <f>TREND(Calcs!$D7:$E7,Calcs!$D3:$E3,BLAPE!M1)*10^12</f>
-        <v>-1024300000000002.9</v>
+        <v>-824760000000000.5</v>
       </c>
       <c r="N2" s="4">
         <f>TREND(Calcs!$D7:$E7,Calcs!$D3:$E3,BLAPE!N1)*10^12</f>
-        <v>-994099999999998.5</v>
+        <v>-825820000000000.38</v>
       </c>
       <c r="O2" s="4">
         <f>TREND(Calcs!$D7:$E7,Calcs!$D3:$E3,BLAPE!O1)*10^12</f>
-        <v>-963900000000001.5</v>
+        <v>-826880000000000.38</v>
       </c>
       <c r="P2" s="4">
         <f>TREND(Calcs!$D7:$E7,Calcs!$D3:$E3,BLAPE!P1)*10^12</f>
-        <v>-933700000000004.38</v>
+        <v>-827940000000000.25</v>
       </c>
       <c r="Q2" s="5">
         <f>TREND(Calcs!$D7:$E7,Calcs!$D3:$E3,BLAPE!Q1)*10^12</f>
-        <v>-903500000000000</v>
+        <v>-829000000000000.25</v>
       </c>
       <c r="R2" s="4">
         <f>TREND(Calcs!$E7:$F7,Calcs!$E3:$F3,BLAPE!R1)*10^12</f>
-        <v>-907631500000001.38</v>
+        <v>-830060000000000.13</v>
       </c>
       <c r="S2" s="4">
         <f>TREND(Calcs!$E7:$F7,Calcs!$E3:$F3,BLAPE!S1)*10^12</f>
-        <v>-911763000000000.88</v>
+        <v>-831120000000000.13</v>
       </c>
       <c r="T2" s="4">
         <f>TREND(Calcs!$E7:$F7,Calcs!$E3:$F3,BLAPE!T1)*10^12</f>
-        <v>-915894500000000.38</v>
+        <v>-832180000000000.5</v>
       </c>
       <c r="U2" s="4">
         <f>TREND(Calcs!$E7:$F7,Calcs!$E3:$F3,BLAPE!U1)*10^12</f>
-        <v>-920025999999999.88</v>
-      </c>
-      <c r="V2" s="11">
+        <v>-833240000000000.5</v>
+      </c>
+      <c r="V2" s="10">
         <f>TREND(Calcs!$E7:$F7,Calcs!$E3:$F3,BLAPE!V1)*10^12</f>
-        <v>-924157499999999.38</v>
-      </c>
-      <c r="W2" s="11">
+        <v>-834300000000000.38</v>
+      </c>
+      <c r="W2" s="10">
         <f>TREND(Calcs!$E7:$F7,Calcs!$E3:$F3,BLAPE!W1)*10^12</f>
-        <v>-928289000000000.63</v>
+        <v>-835360000000000.38</v>
       </c>
       <c r="X2" s="4">
         <f>TREND(Calcs!$E7:$F7,Calcs!$E3:$F3,BLAPE!X1)*10^12</f>
-        <v>-932420500000000.13</v>
+        <v>-836420000000000.25</v>
       </c>
       <c r="Y2" s="4">
         <f>TREND(Calcs!$E7:$F7,Calcs!$E3:$F3,BLAPE!Y1)*10^12</f>
-        <v>-936551999999999.63</v>
+        <v>-837480000000000.25</v>
       </c>
       <c r="Z2" s="4">
         <f>TREND(Calcs!$E7:$F7,Calcs!$E3:$F3,BLAPE!Z1)*10^12</f>
-        <v>-940683499999999.13</v>
+        <v>-838540000000000.25</v>
       </c>
       <c r="AA2" s="4">
         <f>TREND(Calcs!$E7:$F7,Calcs!$E3:$F3,BLAPE!AA1)*10^12</f>
-        <v>-944814999999998.75</v>
+        <v>-839600000000000.13</v>
       </c>
       <c r="AB2" s="4">
         <f>TREND(Calcs!$E7:$F7,Calcs!$E3:$F3,BLAPE!AB1)*10^12</f>
-        <v>-948946500000000</v>
+        <v>-840660000000000.13</v>
       </c>
       <c r="AC2" s="4">
         <f>TREND(Calcs!$E7:$F7,Calcs!$E3:$F3,BLAPE!AC1)*10^12</f>
-        <v>-953077999999999.5</v>
+        <v>-841720000000000</v>
       </c>
       <c r="AD2" s="4">
         <f>TREND(Calcs!$E7:$F7,Calcs!$E3:$F3,BLAPE!AD1)*10^12</f>
-        <v>-957209499999999</v>
+        <v>-842780000000000.38</v>
       </c>
       <c r="AE2" s="4">
         <f>TREND(Calcs!$E7:$F7,Calcs!$E3:$F3,BLAPE!AE1)*10^12</f>
-        <v>-961340999999998.5</v>
+        <v>-843840000000000.38</v>
       </c>
       <c r="AF2" s="4">
         <f>TREND(Calcs!$E7:$F7,Calcs!$E3:$F3,BLAPE!AF1)*10^12</f>
-        <v>-965472499999998</v>
+        <v>-844900000000000.38</v>
       </c>
       <c r="AG2" s="4">
         <f>TREND(Calcs!$E7:$F7,Calcs!$E3:$F3,BLAPE!AG1)*10^12</f>
-        <v>-969603999999999.38</v>
+        <v>-845960000000000.25</v>
       </c>
       <c r="AH2" s="4">
         <f>TREND(Calcs!$E7:$F7,Calcs!$E3:$F3,BLAPE!AH1)*10^12</f>
-        <v>-973735499999998.88</v>
+        <v>-847020000000000.25</v>
       </c>
       <c r="AI2" s="4">
         <f>TREND(Calcs!$E7:$F7,Calcs!$E3:$F3,BLAPE!AI1)*10^12</f>
-        <v>-977866999999998.38</v>
+        <v>-848080000000000.13</v>
       </c>
       <c r="AJ2" s="4">
         <f>TREND(Calcs!$E7:$F7,Calcs!$E3:$F3,BLAPE!AJ1)*10^12</f>
-        <v>-981998499999997.88</v>
+        <v>-849140000000000.13</v>
       </c>
       <c r="AK2" s="4">
         <f>TREND(Calcs!$E7:$F7,Calcs!$E3:$F3,BLAPE!AK1)*10^12</f>
-        <v>-986129999999997.38</v>
+        <v>-850200000000000</v>
       </c>
     </row>
     <row r="3" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="B3">
         <v>0</v>
@@ -1543,7 +1510,7 @@
     </row>
     <row r="4" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="B4">
         <v>0</v>
@@ -1656,7 +1623,7 @@
     </row>
     <row r="5" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="B5">
         <v>0</v>
@@ -1769,7 +1736,7 @@
     </row>
     <row r="6" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="B6">
         <v>0</v>
@@ -1882,7 +1849,7 @@
     </row>
     <row r="7" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="B7">
         <v>0</v>
@@ -1995,7 +1962,7 @@
     </row>
     <row r="8" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="B8">
         <v>0</v>
@@ -2108,7 +2075,7 @@
     </row>
     <row r="9" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B9">
         <v>0</v>
@@ -2221,7 +2188,7 @@
     </row>
     <row r="10" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="B10">
         <v>0</v>
@@ -2334,7 +2301,7 @@
     </row>
     <row r="11" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="B11" s="4">
         <f>B$2*-'data from RPEpUACE'!$B11</f>
@@ -2362,128 +2329,128 @@
       </c>
       <c r="H11" s="4">
         <f>H$2*-'data from RPEpUACE'!$B11</f>
-        <v>372192090644.17133</v>
+        <v>352344597628.60651</v>
       </c>
       <c r="I11" s="4">
         <f>I$2*-'data from RPEpUACE'!$B11</f>
-        <v>392495353646.66467</v>
+        <v>352800367615.53241</v>
       </c>
       <c r="J11" s="4">
         <f>J$2*-'data from RPEpUACE'!$B11</f>
-        <v>412798616649.15802</v>
+        <v>353256137602.45831</v>
       </c>
       <c r="K11" s="4">
         <f>K$2*-'data from RPEpUACE'!$B11</f>
-        <v>433101879651.65137</v>
+        <v>353711907589.38422</v>
       </c>
       <c r="L11" s="4">
         <f>L$2*-'data from RPEpUACE'!$B11</f>
-        <v>453405142654.14471</v>
+        <v>354167677576.31012</v>
       </c>
       <c r="M11" s="4">
         <f>M$2*-'data from RPEpUACE'!$B11</f>
-        <v>440419997743.61475</v>
+        <v>354623447563.23627</v>
       </c>
       <c r="N11" s="4">
         <f>N$2*-'data from RPEpUACE'!$B11</f>
-        <v>427434852833.08167</v>
+        <v>355079217550.16211</v>
       </c>
       <c r="O11" s="4">
         <f>O$2*-'data from RPEpUACE'!$B11</f>
-        <v>414449707922.5517</v>
+        <v>355534987537.08807</v>
       </c>
       <c r="P11" s="4">
         <f>P$2*-'data from RPEpUACE'!$B11</f>
-        <v>401464563012.02173</v>
+        <v>355990757524.01392</v>
       </c>
       <c r="Q11" s="4">
         <f>Q$2*-'data from RPEpUACE'!$B11</f>
-        <v>388479418101.48865</v>
+        <v>356446527510.93988</v>
       </c>
       <c r="R11" s="4">
         <f>R$2*-'data from RPEpUACE'!$B11</f>
-        <v>390255846121.28589</v>
+        <v>356902297497.86572</v>
       </c>
       <c r="S11" s="4">
         <f>S$2*-'data from RPEpUACE'!$B11</f>
-        <v>392032274141.0824</v>
+        <v>357358067484.79169</v>
       </c>
       <c r="T11" s="4">
         <f>T$2*-'data from RPEpUACE'!$B11</f>
-        <v>393808702160.87885</v>
+        <v>357813837471.71777</v>
       </c>
       <c r="U11" s="4">
         <f>U$2*-'data from RPEpUACE'!$B11</f>
-        <v>395585130180.67529</v>
+        <v>358269607458.64368</v>
       </c>
       <c r="V11" s="4">
         <f>V$2*-'data from RPEpUACE'!$B11</f>
-        <v>397361558200.47174</v>
+        <v>358725377445.56958</v>
       </c>
       <c r="W11" s="4">
         <f>W$2*-'data from RPEpUACE'!$B11</f>
-        <v>399137986220.26898</v>
+        <v>359181147432.49548</v>
       </c>
       <c r="X11" s="4">
         <f>X$2*-'data from RPEpUACE'!$B11</f>
-        <v>400914414240.06543</v>
+        <v>359636917419.42139</v>
       </c>
       <c r="Y11" s="4">
         <f>Y$2*-'data from RPEpUACE'!$B11</f>
-        <v>402690842259.86194</v>
+        <v>360092687406.34729</v>
       </c>
       <c r="Z11" s="4">
         <f>Z$2*-'data from RPEpUACE'!$B11</f>
-        <v>404467270279.65839</v>
+        <v>360548457393.27325</v>
       </c>
       <c r="AA11" s="4">
         <f>AA$2*-'data from RPEpUACE'!$B11</f>
-        <v>406243698299.4549</v>
+        <v>361004227380.1991</v>
       </c>
       <c r="AB11" s="4">
         <f>AB$2*-'data from RPEpUACE'!$B11</f>
-        <v>408020126319.25214</v>
+        <v>361459997367.12506</v>
       </c>
       <c r="AC11" s="4">
         <f>AC$2*-'data from RPEpUACE'!$B11</f>
-        <v>409796554339.04858</v>
+        <v>361915767354.0509</v>
       </c>
       <c r="AD11" s="4">
         <f>AD$2*-'data from RPEpUACE'!$B11</f>
-        <v>411572982358.84503</v>
+        <v>362371537340.97699</v>
       </c>
       <c r="AE11" s="4">
         <f>AE$2*-'data from RPEpUACE'!$B11</f>
-        <v>413349410378.64148</v>
+        <v>362827307327.90295</v>
       </c>
       <c r="AF11" s="4">
         <f>AF$2*-'data from RPEpUACE'!$B11</f>
-        <v>415125838398.43799</v>
+        <v>363283077314.82886</v>
       </c>
       <c r="AG11" s="4">
         <f>AG$2*-'data from RPEpUACE'!$B11</f>
-        <v>416902266418.23523</v>
+        <v>363738847301.75476</v>
       </c>
       <c r="AH11" s="4">
         <f>AH$2*-'data from RPEpUACE'!$B11</f>
-        <v>418678694438.03168</v>
+        <v>364194617288.68066</v>
       </c>
       <c r="AI11" s="4">
         <f>AI$2*-'data from RPEpUACE'!$B11</f>
-        <v>420455122457.82819</v>
+        <v>364650387275.60657</v>
       </c>
       <c r="AJ11" s="4">
         <f>AJ$2*-'data from RPEpUACE'!$B11</f>
-        <v>422231550477.62463</v>
+        <v>365106157262.53247</v>
       </c>
       <c r="AK11" s="4">
         <f>AK$2*-'data from RPEpUACE'!$B11</f>
-        <v>424007978497.42108</v>
+        <v>365561927249.45837</v>
       </c>
     </row>
     <row r="12" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="B12" s="4">
         <f>B$2*-'data from RPEpUACE'!$B12</f>
@@ -2511,128 +2478,128 @@
       </c>
       <c r="H12" s="4">
         <f>H$2*-'data from RPEpUACE'!$B12</f>
-        <v>30299948942.914848</v>
+        <v>28684175689.980755</v>
       </c>
       <c r="I12" s="4">
         <f>I$2*-'data from RPEpUACE'!$B12</f>
-        <v>31952826174.361073</v>
+        <v>28721279668.492676</v>
       </c>
       <c r="J12" s="4">
         <f>J$2*-'data from RPEpUACE'!$B12</f>
-        <v>33605703405.807297</v>
+        <v>28758383647.004593</v>
       </c>
       <c r="K12" s="4">
         <f>K$2*-'data from RPEpUACE'!$B12</f>
-        <v>35258580637.253525</v>
+        <v>28795487625.516518</v>
       </c>
       <c r="L12" s="4">
         <f>L$2*-'data from RPEpUACE'!$B12</f>
-        <v>36911457868.699745</v>
+        <v>28832591604.028435</v>
       </c>
       <c r="M12" s="4">
         <f>M$2*-'data from RPEpUACE'!$B12</f>
-        <v>35854344518.643204</v>
+        <v>28869695582.540375</v>
       </c>
       <c r="N12" s="4">
         <f>N$2*-'data from RPEpUACE'!$B12</f>
-        <v>34797231168.586403</v>
+        <v>28906799561.052292</v>
       </c>
       <c r="O12" s="4">
         <f>O$2*-'data from RPEpUACE'!$B12</f>
-        <v>33740117818.529865</v>
+        <v>28943903539.564213</v>
       </c>
       <c r="P12" s="4">
         <f>P$2*-'data from RPEpUACE'!$B12</f>
-        <v>32683004468.47332</v>
+        <v>28981007518.07613</v>
       </c>
       <c r="Q12" s="4">
         <f>Q$2*-'data from RPEpUACE'!$B12</f>
-        <v>31625891118.416523</v>
+        <v>29018111496.588051</v>
       </c>
       <c r="R12" s="4">
         <f>R$2*-'data from RPEpUACE'!$B12</f>
-        <v>31770509125.229782</v>
+        <v>29055215475.099968</v>
       </c>
       <c r="S12" s="4">
         <f>S$2*-'data from RPEpUACE'!$B12</f>
-        <v>31915127132.04298</v>
+        <v>29092319453.611893</v>
       </c>
       <c r="T12" s="4">
         <f>T$2*-'data from RPEpUACE'!$B12</f>
-        <v>32059745138.856174</v>
+        <v>29129423432.123825</v>
       </c>
       <c r="U12" s="4">
         <f>U$2*-'data from RPEpUACE'!$B12</f>
-        <v>32204363145.669369</v>
+        <v>29166527410.63575</v>
       </c>
       <c r="V12" s="4">
         <f>V$2*-'data from RPEpUACE'!$B12</f>
-        <v>32348981152.482567</v>
+        <v>29203631389.147667</v>
       </c>
       <c r="W12" s="4">
         <f>W$2*-'data from RPEpUACE'!$B12</f>
-        <v>32493599159.295822</v>
+        <v>29240735367.659588</v>
       </c>
       <c r="X12" s="4">
         <f>X$2*-'data from RPEpUACE'!$B12</f>
-        <v>32638217166.109016</v>
+        <v>29277839346.171505</v>
       </c>
       <c r="Y12" s="4">
         <f>Y$2*-'data from RPEpUACE'!$B12</f>
-        <v>32782835172.922215</v>
+        <v>29314943324.68343</v>
       </c>
       <c r="Z12" s="4">
         <f>Z$2*-'data from RPEpUACE'!$B12</f>
-        <v>32927453179.735409</v>
+        <v>29352047303.195351</v>
       </c>
       <c r="AA12" s="4">
         <f>AA$2*-'data from RPEpUACE'!$B12</f>
-        <v>33072071186.548607</v>
+        <v>29389151281.707268</v>
       </c>
       <c r="AB12" s="4">
         <f>AB$2*-'data from RPEpUACE'!$B12</f>
-        <v>33216689193.361866</v>
+        <v>29426255260.219189</v>
       </c>
       <c r="AC12" s="4">
         <f>AC$2*-'data from RPEpUACE'!$B12</f>
-        <v>33361307200.17506</v>
+        <v>29463359238.731106</v>
       </c>
       <c r="AD12" s="4">
         <f>AD$2*-'data from RPEpUACE'!$B12</f>
-        <v>33505925206.988255</v>
+        <v>29500463217.243042</v>
       </c>
       <c r="AE12" s="4">
         <f>AE$2*-'data from RPEpUACE'!$B12</f>
-        <v>33650543213.801453</v>
+        <v>29537567195.754963</v>
       </c>
       <c r="AF12" s="4">
         <f>AF$2*-'data from RPEpUACE'!$B12</f>
-        <v>33795161220.614647</v>
+        <v>29574671174.266888</v>
       </c>
       <c r="AG12" s="4">
         <f>AG$2*-'data from RPEpUACE'!$B12</f>
-        <v>33939779227.427906</v>
+        <v>29611775152.778805</v>
       </c>
       <c r="AH12" s="4">
         <f>AH$2*-'data from RPEpUACE'!$B12</f>
-        <v>34084397234.241104</v>
+        <v>29648879131.290726</v>
       </c>
       <c r="AI12" s="4">
         <f>AI$2*-'data from RPEpUACE'!$B12</f>
-        <v>34229015241.054298</v>
+        <v>29685983109.802643</v>
       </c>
       <c r="AJ12" s="4">
         <f>AJ$2*-'data from RPEpUACE'!$B12</f>
-        <v>34373633247.867493</v>
+        <v>29723087088.314564</v>
       </c>
       <c r="AK12" s="4">
         <f>AK$2*-'data from RPEpUACE'!$B12</f>
-        <v>34518251254.680687</v>
+        <v>29760191066.826485</v>
       </c>
     </row>
     <row r="13" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="B13">
         <v>0</v>

</xml_diff>

<commit_message>
Update rebound pollutant emissions for LULUCF
</commit_message>
<xml_diff>
--- a/InputData/land/BLAPE/BAU LULUCF Anthro Pollutant Emis.xlsx
+++ b/InputData/land/BLAPE/BAU LULUCF Anthro Pollutant Emis.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23801"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rorvis\Dropbox (Energy InNovation)\My Documents\Energy Policy Solutions\US\Models\eps-us\InputData\land\BLAPE\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MeganM\Documents\eps-us\InputData\land\BLAPE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9B6FDE4-7C6E-4C9F-A4A8-79AB3428627D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -19,7 +18,7 @@
     <sheet name="data from RPEpUACE" sheetId="4" r:id="rId4"/>
     <sheet name="BLAPE" sheetId="3" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -35,14 +34,14 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
   <futureMetadata name="XLDAPR" count="1">
     <bk>
       <extLst>
-        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+        <ext xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray" uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
           <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
         </ext>
       </extLst>
@@ -57,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="55">
   <si>
     <t>Source:</t>
   </si>
@@ -207,12 +206,27 @@
   </si>
   <si>
     <t>These are relatively constant.</t>
+  </si>
+  <si>
+    <t>CO2 Sequestration</t>
+  </si>
+  <si>
+    <t>U.S. State Department</t>
+  </si>
+  <si>
+    <t>Second Biennial Report of the United States of America</t>
+  </si>
+  <si>
+    <t>https://unfccc.int/files/national_reports/biennial_reports_and_iar/submitted_biennial_reports/application/pdf/2016_second_biennial_report_of_the_united_states_.pdf</t>
+  </si>
+  <si>
+    <t>Page 34, Table 3</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -410,23 +424,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -462,23 +459,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -654,25 +634,25 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B22"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+      <selection activeCell="A16" sqref="A16:XFD16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="9.42578125" customWidth="1"/>
-    <col min="2" max="2" width="51.5703125" customWidth="1"/>
+    <col min="1" max="1" width="9.3984375" customWidth="1"/>
+    <col min="2" max="2" width="51.59765625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
@@ -680,57 +660,87 @@
         <v>43</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
       <c r="B4" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
       <c r="B5" s="6">
         <v>2021</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
       <c r="B6" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.45">
       <c r="B7" s="2" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.45">
       <c r="B8" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.45">
       <c r="B10" s="12" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="B11" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="B12" s="6">
+        <v>2016</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="B13" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="B14" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="B15" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="B17" s="12" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="11" spans="1:2" s="16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="13" t="s">
+    <row r="18" spans="1:2" s="16" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="B18" s="13" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="12" spans="1:2" s="16" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="13" spans="1:2" s="16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B13"/>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A20" s="1" t="s">
+    <row r="19" spans="1:2" s="16" customFormat="1" x14ac:dyDescent="0.45"/>
+    <row r="20" spans="1:2" s="16" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="B20"/>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A27" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A28" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A29" t="s">
         <v>49</v>
       </c>
     </row>
@@ -741,29 +751,29 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="63.28515625" customWidth="1"/>
+    <col min="1" max="1" width="63.265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.45">
       <c r="B3">
         <v>2015</v>
       </c>
@@ -780,7 +790,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>1</v>
       </c>
@@ -804,7 +814,7 @@
         <v>-850.2</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -828,7 +838,7 @@
         <v>-850.2</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>4</v>
       </c>
@@ -853,22 +863,22 @@
         <v>-850.2</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.45">
       <c r="G11" s="15" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
         <v>40</v>
       </c>
@@ -891,7 +901,7 @@
         <v>2020</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
         <v>42</v>
       </c>
@@ -929,19 +939,19 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{748C1EED-5369-4626-8108-4C2C32A7C6AB}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="21.5703125" customWidth="1"/>
+    <col min="1" max="1" width="21.59765625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>38</v>
       </c>
@@ -967,7 +977,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>39</v>
       </c>
@@ -1000,22 +1010,24 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B13"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:B13"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="2" max="2" width="23" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
       <c r="B1" s="11" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>24</v>
       </c>
@@ -1023,7 +1035,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>25</v>
       </c>
@@ -1031,7 +1043,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>26</v>
       </c>
@@ -1039,7 +1051,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>27</v>
       </c>
@@ -1047,7 +1059,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>28</v>
       </c>
@@ -1055,7 +1067,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>29</v>
       </c>
@@ -1063,7 +1075,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>30</v>
       </c>
@@ -1071,7 +1083,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>31</v>
       </c>
@@ -1079,7 +1091,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
         <v>32</v>
       </c>
@@ -1087,23 +1099,23 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
         <v>33</v>
       </c>
       <c r="B11" s="4">
-        <v>4.2997168577917945E-4</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+        <v>6.6417418588509813E-4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
         <v>34</v>
       </c>
       <c r="B12" s="4">
-        <v>3.5003753313133949E-5</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+        <v>3.8529345186784264E-5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
         <v>35</v>
       </c>
@@ -1117,7 +1129,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="3"/>
   </sheetPr>
@@ -1127,13 +1139,13 @@
       <selection activeCell="AK2" sqref="AK2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="16.7109375" customWidth="1"/>
-    <col min="2" max="17" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.73046875" customWidth="1"/>
+    <col min="2" max="17" width="11.265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:37" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>8</v>
       </c>
@@ -1246,7 +1258,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="2" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:37" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -1395,7 +1407,7 @@
         <v>-850200000000000</v>
       </c>
     </row>
-    <row r="3" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:37" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>13</v>
       </c>
@@ -1508,7 +1520,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:37" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>14</v>
       </c>
@@ -1621,7 +1633,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:37" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>15</v>
       </c>
@@ -1734,7 +1746,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:37" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>16</v>
       </c>
@@ -1847,7 +1859,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:37" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>17</v>
       </c>
@@ -1960,7 +1972,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:37" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>18</v>
       </c>
@@ -2073,7 +2085,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:37" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>19</v>
       </c>
@@ -2186,7 +2198,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:37" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
         <v>20</v>
       </c>
@@ -2299,305 +2311,305 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:37" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
         <v>21</v>
       </c>
       <c r="B11" s="4">
         <f>B$2*-'data from RPEpUACE'!$B11</f>
-        <v>408043129804.43817</v>
+        <v>630301302404.95325</v>
       </c>
       <c r="C11" s="4">
         <f>C$2*-'data from RPEpUACE'!$B11</f>
-        <v>396812269371.888</v>
+        <v>612953072669.63757</v>
       </c>
       <c r="D11" s="4">
         <f>D$2*-'data from RPEpUACE'!$B11</f>
-        <v>385581408939.33472</v>
+        <v>595604842934.31714</v>
       </c>
       <c r="E11" s="4">
         <f>E$2*-'data from RPEpUACE'!$B11</f>
-        <v>374350548506.78143</v>
+        <v>578256613198.99658</v>
       </c>
       <c r="F11" s="4">
         <f>F$2*-'data from RPEpUACE'!$B11</f>
-        <v>363119688074.2312</v>
+        <v>560908383463.68091</v>
       </c>
       <c r="G11" s="4">
         <f>G$2*-'data from RPEpUACE'!$B11</f>
-        <v>351888827641.67792</v>
+        <v>543560153728.36041</v>
       </c>
       <c r="H11" s="4">
         <f>H$2*-'data from RPEpUACE'!$B11</f>
-        <v>352344597628.60651</v>
+        <v>544264178365.40265</v>
       </c>
       <c r="I11" s="4">
         <f>I$2*-'data from RPEpUACE'!$B11</f>
-        <v>352800367615.53241</v>
+        <v>544968203002.44086</v>
       </c>
       <c r="J11" s="4">
         <f>J$2*-'data from RPEpUACE'!$B11</f>
-        <v>353256137602.45831</v>
+        <v>545672227639.479</v>
       </c>
       <c r="K11" s="4">
         <f>K$2*-'data from RPEpUACE'!$B11</f>
-        <v>353711907589.38422</v>
+        <v>546376252276.51721</v>
       </c>
       <c r="L11" s="4">
         <f>L$2*-'data from RPEpUACE'!$B11</f>
-        <v>354167677576.31012</v>
+        <v>547080276913.5553</v>
       </c>
       <c r="M11" s="4">
         <f>M$2*-'data from RPEpUACE'!$B11</f>
-        <v>354623447563.23627</v>
+        <v>547784301550.59387</v>
       </c>
       <c r="N11" s="4">
         <f>N$2*-'data from RPEpUACE'!$B11</f>
-        <v>355079217550.16211</v>
+        <v>548488326187.63196</v>
       </c>
       <c r="O11" s="4">
         <f>O$2*-'data from RPEpUACE'!$B11</f>
-        <v>355534987537.08807</v>
+        <v>549192350824.67017</v>
       </c>
       <c r="P11" s="4">
         <f>P$2*-'data from RPEpUACE'!$B11</f>
-        <v>355990757524.01392</v>
+        <v>549896375461.70825</v>
       </c>
       <c r="Q11" s="4">
         <f>Q$2*-'data from RPEpUACE'!$B11</f>
-        <v>356446527510.93988</v>
+        <v>550600400098.74646</v>
       </c>
       <c r="R11" s="4">
         <f>R$2*-'data from RPEpUACE'!$B11</f>
-        <v>356902297497.86572</v>
+        <v>551304424735.78467</v>
       </c>
       <c r="S11" s="4">
         <f>S$2*-'data from RPEpUACE'!$B11</f>
-        <v>357358067484.79169</v>
+        <v>552008449372.82288</v>
       </c>
       <c r="T11" s="4">
         <f>T$2*-'data from RPEpUACE'!$B11</f>
-        <v>357813837471.71777</v>
+        <v>552712474009.86133</v>
       </c>
       <c r="U11" s="4">
         <f>U$2*-'data from RPEpUACE'!$B11</f>
-        <v>358269607458.64368</v>
+        <v>553416498646.89954</v>
       </c>
       <c r="V11" s="4">
         <f>V$2*-'data from RPEpUACE'!$B11</f>
-        <v>358725377445.56958</v>
+        <v>554120523283.93762</v>
       </c>
       <c r="W11" s="4">
         <f>W$2*-'data from RPEpUACE'!$B11</f>
-        <v>359181147432.49548</v>
+        <v>554824547920.97583</v>
       </c>
       <c r="X11" s="4">
         <f>X$2*-'data from RPEpUACE'!$B11</f>
-        <v>359636917419.42139</v>
+        <v>555528572558.01392</v>
       </c>
       <c r="Y11" s="4">
         <f>Y$2*-'data from RPEpUACE'!$B11</f>
-        <v>360092687406.34729</v>
+        <v>556232597195.05212</v>
       </c>
       <c r="Z11" s="4">
         <f>Z$2*-'data from RPEpUACE'!$B11</f>
-        <v>360548457393.27325</v>
+        <v>556936621832.09033</v>
       </c>
       <c r="AA11" s="4">
         <f>AA$2*-'data from RPEpUACE'!$B11</f>
-        <v>361004227380.1991</v>
+        <v>557640646469.12842</v>
       </c>
       <c r="AB11" s="4">
         <f>AB$2*-'data from RPEpUACE'!$B11</f>
-        <v>361459997367.12506</v>
+        <v>558344671106.16663</v>
       </c>
       <c r="AC11" s="4">
         <f>AC$2*-'data from RPEpUACE'!$B11</f>
-        <v>361915767354.0509</v>
+        <v>559048695743.20483</v>
       </c>
       <c r="AD11" s="4">
         <f>AD$2*-'data from RPEpUACE'!$B11</f>
-        <v>362371537340.97699</v>
+        <v>559752720380.24329</v>
       </c>
       <c r="AE11" s="4">
         <f>AE$2*-'data from RPEpUACE'!$B11</f>
-        <v>362827307327.90295</v>
+        <v>560456745017.28149</v>
       </c>
       <c r="AF11" s="4">
         <f>AF$2*-'data from RPEpUACE'!$B11</f>
-        <v>363283077314.82886</v>
+        <v>561160769654.3197</v>
       </c>
       <c r="AG11" s="4">
         <f>AG$2*-'data from RPEpUACE'!$B11</f>
-        <v>363738847301.75476</v>
+        <v>561864794291.35779</v>
       </c>
       <c r="AH11" s="4">
         <f>AH$2*-'data from RPEpUACE'!$B11</f>
-        <v>364194617288.68066</v>
+        <v>562568818928.396</v>
       </c>
       <c r="AI11" s="4">
         <f>AI$2*-'data from RPEpUACE'!$B11</f>
-        <v>364650387275.60657</v>
+        <v>563272843565.43408</v>
       </c>
       <c r="AJ11" s="4">
         <f>AJ$2*-'data from RPEpUACE'!$B11</f>
-        <v>365106157262.53247</v>
+        <v>563976868202.47229</v>
       </c>
       <c r="AK11" s="4">
         <f>AK$2*-'data from RPEpUACE'!$B11</f>
-        <v>365561927249.45837</v>
-      </c>
-    </row>
-    <row r="12" spans="1:37" x14ac:dyDescent="0.25">
+        <v>564680892839.51038</v>
+      </c>
+    </row>
+    <row r="12" spans="1:37" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
         <v>22</v>
       </c>
       <c r="B12" s="4">
         <f>B$2*-'data from RPEpUACE'!$B12</f>
-        <v>33218561894.163864</v>
+        <v>36564348582.257988</v>
       </c>
       <c r="C12" s="4">
         <f>C$2*-'data from RPEpUACE'!$B12</f>
-        <v>32304263857.624966</v>
+        <v>35557962085.979362</v>
       </c>
       <c r="D12" s="4">
         <f>D$2*-'data from RPEpUACE'!$B12</f>
-        <v>31389965821.085815</v>
+        <v>34551575589.700455</v>
       </c>
       <c r="E12" s="4">
         <f>E$2*-'data from RPEpUACE'!$B12</f>
-        <v>30475667784.546665</v>
+        <v>33545189093.421547</v>
       </c>
       <c r="F12" s="4">
         <f>F$2*-'data from RPEpUACE'!$B12</f>
-        <v>29561369748.007767</v>
+        <v>32538802597.142921</v>
       </c>
       <c r="G12" s="4">
         <f>G$2*-'data from RPEpUACE'!$B12</f>
-        <v>28647071711.468616</v>
+        <v>31532416100.864014</v>
       </c>
       <c r="H12" s="4">
         <f>H$2*-'data from RPEpUACE'!$B12</f>
-        <v>28684175689.980755</v>
+        <v>31573257206.762241</v>
       </c>
       <c r="I12" s="4">
         <f>I$2*-'data from RPEpUACE'!$B12</f>
-        <v>28721279668.492676</v>
+        <v>31614098312.660233</v>
       </c>
       <c r="J12" s="4">
         <f>J$2*-'data from RPEpUACE'!$B12</f>
-        <v>28758383647.004593</v>
+        <v>31654939418.55822</v>
       </c>
       <c r="K12" s="4">
         <f>K$2*-'data from RPEpUACE'!$B12</f>
-        <v>28795487625.516518</v>
+        <v>31695780524.456211</v>
       </c>
       <c r="L12" s="4">
         <f>L$2*-'data from RPEpUACE'!$B12</f>
-        <v>28832591604.028435</v>
+        <v>31736621630.354198</v>
       </c>
       <c r="M12" s="4">
         <f>M$2*-'data from RPEpUACE'!$B12</f>
-        <v>28869695582.540375</v>
+        <v>31777462736.252209</v>
       </c>
       <c r="N12" s="4">
         <f>N$2*-'data from RPEpUACE'!$B12</f>
-        <v>28906799561.052292</v>
+        <v>31818303842.150196</v>
       </c>
       <c r="O12" s="4">
         <f>O$2*-'data from RPEpUACE'!$B12</f>
-        <v>28943903539.564213</v>
+        <v>31859144948.048187</v>
       </c>
       <c r="P12" s="4">
         <f>P$2*-'data from RPEpUACE'!$B12</f>
-        <v>28981007518.07613</v>
+        <v>31899986053.946175</v>
       </c>
       <c r="Q12" s="4">
         <f>Q$2*-'data from RPEpUACE'!$B12</f>
-        <v>29018111496.588051</v>
+        <v>31940827159.844166</v>
       </c>
       <c r="R12" s="4">
         <f>R$2*-'data from RPEpUACE'!$B12</f>
-        <v>29055215475.099968</v>
+        <v>31981668265.742149</v>
       </c>
       <c r="S12" s="4">
         <f>S$2*-'data from RPEpUACE'!$B12</f>
-        <v>29092319453.611893</v>
+        <v>32022509371.640141</v>
       </c>
       <c r="T12" s="4">
         <f>T$2*-'data from RPEpUACE'!$B12</f>
-        <v>29129423432.123825</v>
+        <v>32063350477.538147</v>
       </c>
       <c r="U12" s="4">
         <f>U$2*-'data from RPEpUACE'!$B12</f>
-        <v>29166527410.63575</v>
+        <v>32104191583.436138</v>
       </c>
       <c r="V12" s="4">
         <f>V$2*-'data from RPEpUACE'!$B12</f>
-        <v>29203631389.147667</v>
+        <v>32145032689.334126</v>
       </c>
       <c r="W12" s="4">
         <f>W$2*-'data from RPEpUACE'!$B12</f>
-        <v>29240735367.659588</v>
+        <v>32185873795.232117</v>
       </c>
       <c r="X12" s="4">
         <f>X$2*-'data from RPEpUACE'!$B12</f>
-        <v>29277839346.171505</v>
+        <v>32226714901.130104</v>
       </c>
       <c r="Y12" s="4">
         <f>Y$2*-'data from RPEpUACE'!$B12</f>
-        <v>29314943324.68343</v>
+        <v>32267556007.028095</v>
       </c>
       <c r="Z12" s="4">
         <f>Z$2*-'data from RPEpUACE'!$B12</f>
-        <v>29352047303.195351</v>
+        <v>32308397112.926086</v>
       </c>
       <c r="AA12" s="4">
         <f>AA$2*-'data from RPEpUACE'!$B12</f>
-        <v>29389151281.707268</v>
+        <v>32349238218.824074</v>
       </c>
       <c r="AB12" s="4">
         <f>AB$2*-'data from RPEpUACE'!$B12</f>
-        <v>29426255260.219189</v>
+        <v>32390079324.722065</v>
       </c>
       <c r="AC12" s="4">
         <f>AC$2*-'data from RPEpUACE'!$B12</f>
-        <v>29463359238.731106</v>
+        <v>32430920430.620049</v>
       </c>
       <c r="AD12" s="4">
         <f>AD$2*-'data from RPEpUACE'!$B12</f>
-        <v>29500463217.243042</v>
+        <v>32471761536.518055</v>
       </c>
       <c r="AE12" s="4">
         <f>AE$2*-'data from RPEpUACE'!$B12</f>
-        <v>29537567195.754963</v>
+        <v>32512602642.416046</v>
       </c>
       <c r="AF12" s="4">
         <f>AF$2*-'data from RPEpUACE'!$B12</f>
-        <v>29574671174.266888</v>
+        <v>32553443748.314037</v>
       </c>
       <c r="AG12" s="4">
         <f>AG$2*-'data from RPEpUACE'!$B12</f>
-        <v>29611775152.778805</v>
+        <v>32594284854.212025</v>
       </c>
       <c r="AH12" s="4">
         <f>AH$2*-'data from RPEpUACE'!$B12</f>
-        <v>29648879131.290726</v>
+        <v>32635125960.110016</v>
       </c>
       <c r="AI12" s="4">
         <f>AI$2*-'data from RPEpUACE'!$B12</f>
-        <v>29685983109.802643</v>
+        <v>32675967066.008003</v>
       </c>
       <c r="AJ12" s="4">
         <f>AJ$2*-'data from RPEpUACE'!$B12</f>
-        <v>29723087088.314564</v>
+        <v>32716808171.905994</v>
       </c>
       <c r="AK12" s="4">
         <f>AK$2*-'data from RPEpUACE'!$B12</f>
-        <v>29760191066.826485</v>
-      </c>
-    </row>
-    <row r="13" spans="1:37" x14ac:dyDescent="0.25">
+        <v>32757649277.803982</v>
+      </c>
+    </row>
+    <row r="13" spans="1:37" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
         <v>11</v>
       </c>

</xml_diff>